<commit_message>
add GEO background information, update ArrayExpress tag and MIAPPE template name
</commit_message>
<xml_diff>
--- a/templates/dataplant/ArrayExpress_-_Plant_sample.xlsx
+++ b/templates/dataplant/ArrayExpress_-_Plant_sample.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="72">
   <si>
     <t>TEMPLATE</t>
   </si>
@@ -83,6 +83,9 @@
     <t>Genomics</t>
   </si>
   <si>
+    <t>Transcriptomics</t>
+  </si>
+  <si>
     <t>mandatory</t>
   </si>
   <si>
@@ -96,6 +99,9 @@
   </si>
   <si>
     <t>http://purl.obolibrary.org/obo/NCIT_C84343</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C153189</t>
   </si>
   <si>
     <t>Tags Term Source REF</t>
@@ -629,7 +635,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:F27"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -713,7 +719,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -729,105 +735,114 @@
       <c r="E13" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B14" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C14" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D14" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="E14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B15" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C15" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D15" t="s">
-        <v>29</v>
+        <v>31</v>
+      </c>
+      <c r="E15" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B17" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B18" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B20" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B24" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -843,73 +858,73 @@
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="E1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="F1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="G1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="H1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="I1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="J1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="K1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="L1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="M1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="N1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="O1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="P1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="Q1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="R1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="S1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="T1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="U1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="V1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="W1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add protocol columns to arrayexpress templates
</commit_message>
<xml_diff>
--- a/templates/dataplant/ArrayExpress_-_Plant_sample.xlsx
+++ b/templates/dataplant/ArrayExpress_-_Plant_sample.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="77">
   <si>
     <t>TEMPLATE</t>
   </si>
@@ -32,7 +32,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>1.0.0</t>
+    <t>1.0.1</t>
   </si>
   <si>
     <t>Description</t>
@@ -164,6 +164,18 @@
     <t>Input [Source Name]</t>
   </si>
   <si>
+    <t>Protocol Type</t>
+  </si>
+  <si>
+    <t>Term Source REF (DPBO:1000161)</t>
+  </si>
+  <si>
+    <t>Term Accession Number (DPBO:1000161)</t>
+  </si>
+  <si>
+    <t>Protocol REF</t>
+  </si>
+  <si>
     <t>Characteristic [Organism]</t>
   </si>
   <si>
@@ -228,6 +240,9 @@
   </si>
   <si>
     <t>Output [Sample Name]</t>
+  </si>
+  <si>
+    <t/>
   </si>
 </sst>
 </file>
@@ -283,8 +298,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" name="annotationTable" displayName="annotationTable" ref="A1:W1" totalsRowShown="1" headerRowCount="1">
-  <autoFilter ref="A1:W1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" name="annotationTable" displayName="annotationTable" ref="A1:AA2" totalsRowShown="1" headerRowCount="1">
+  <autoFilter ref="A1:AA2">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -308,31 +323,39 @@
     <filterColumn colId="20" hiddenButton="1"/>
     <filterColumn colId="21" hiddenButton="1"/>
     <filterColumn colId="22" hiddenButton="1"/>
+    <filterColumn colId="23" hiddenButton="1"/>
+    <filterColumn colId="24" hiddenButton="1"/>
+    <filterColumn colId="25" hiddenButton="1"/>
+    <filterColumn colId="26" hiddenButton="1"/>
   </autoFilter>
-  <tableColumns count="23">
+  <tableColumns count="27">
     <tableColumn id="1" name="Input [Source Name]" totalsRowLabel="Total"/>
-    <tableColumn id="2" name="Characteristic [Organism]" totalsRowFunction="none"/>
-    <tableColumn id="3" name="Term Source REF (MIAPPE:0041)" totalsRowFunction="none"/>
-    <tableColumn id="4" name="Term Accession Number (MIAPPE:0041)" totalsRowFunction="none"/>
-    <tableColumn id="5" name="Characteristic [Variety]" totalsRowFunction="none"/>
-    <tableColumn id="6" name="Term Source REF (NCIT:C62709)" totalsRowFunction="none"/>
-    <tableColumn id="7" name="Term Accession Number (NCIT:C62709)" totalsRowFunction="none"/>
-    <tableColumn id="8" name="Characteristic [age]" totalsRowFunction="none"/>
-    <tableColumn id="9" name="Term Source REF (EFO:0000246)" totalsRowFunction="none"/>
-    <tableColumn id="10" name="Term Accession Number (EFO:0000246)" totalsRowFunction="none"/>
-    <tableColumn id="11" name="Characteristic [developmental stage]" totalsRowFunction="none"/>
-    <tableColumn id="12" name="Term Source REF (EFO:0000399)" totalsRowFunction="none"/>
-    <tableColumn id="13" name="Term Accession Number (EFO:0000399)" totalsRowFunction="none"/>
-    <tableColumn id="14" name="Characteristic [Genotype]" totalsRowFunction="none"/>
-    <tableColumn id="15" name="Term Source REF (NCIT:C16631)" totalsRowFunction="none"/>
-    <tableColumn id="16" name="Term Accession Number (NCIT:C16631)" totalsRowFunction="none"/>
-    <tableColumn id="17" name="Characteristic [organism part]" totalsRowFunction="none"/>
-    <tableColumn id="18" name="Term Source REF (EFO:0000635)" totalsRowFunction="none"/>
-    <tableColumn id="19" name="Term Accession Number (EFO:0000635)" totalsRowFunction="none"/>
-    <tableColumn id="20" name="Characteristic [Material]" totalsRowFunction="none"/>
-    <tableColumn id="21" name="Term Source REF (NCIT:C48187)" totalsRowFunction="none"/>
-    <tableColumn id="22" name="Term Accession Number (NCIT:C48187)" totalsRowFunction="none"/>
-    <tableColumn id="23" name="Output [Sample Name]" totalsRowFunction="none"/>
+    <tableColumn id="2" name="Protocol Type" totalsRowFunction="none"/>
+    <tableColumn id="3" name="Term Source REF (DPBO:1000161)" totalsRowFunction="none"/>
+    <tableColumn id="4" name="Term Accession Number (DPBO:1000161)" totalsRowFunction="none"/>
+    <tableColumn id="5" name="Protocol REF" totalsRowFunction="none"/>
+    <tableColumn id="6" name="Characteristic [Organism]" totalsRowFunction="none"/>
+    <tableColumn id="7" name="Term Source REF (MIAPPE:0041)" totalsRowFunction="none"/>
+    <tableColumn id="8" name="Term Accession Number (MIAPPE:0041)" totalsRowFunction="none"/>
+    <tableColumn id="9" name="Characteristic [Variety]" totalsRowFunction="none"/>
+    <tableColumn id="10" name="Term Source REF (NCIT:C62709)" totalsRowFunction="none"/>
+    <tableColumn id="11" name="Term Accession Number (NCIT:C62709)" totalsRowFunction="none"/>
+    <tableColumn id="12" name="Characteristic [age]" totalsRowFunction="none"/>
+    <tableColumn id="13" name="Term Source REF (EFO:0000246)" totalsRowFunction="none"/>
+    <tableColumn id="14" name="Term Accession Number (EFO:0000246)" totalsRowFunction="none"/>
+    <tableColumn id="15" name="Characteristic [developmental stage]" totalsRowFunction="none"/>
+    <tableColumn id="16" name="Term Source REF (EFO:0000399)" totalsRowFunction="none"/>
+    <tableColumn id="17" name="Term Accession Number (EFO:0000399)" totalsRowFunction="none"/>
+    <tableColumn id="18" name="Characteristic [Genotype]" totalsRowFunction="none"/>
+    <tableColumn id="19" name="Term Source REF (NCIT:C16631)" totalsRowFunction="none"/>
+    <tableColumn id="20" name="Term Accession Number (NCIT:C16631)" totalsRowFunction="none"/>
+    <tableColumn id="21" name="Characteristic [organism part]" totalsRowFunction="none"/>
+    <tableColumn id="22" name="Term Source REF (EFO:0000635)" totalsRowFunction="none"/>
+    <tableColumn id="23" name="Term Accession Number (EFO:0000635)" totalsRowFunction="none"/>
+    <tableColumn id="24" name="Characteristic [Material]" totalsRowFunction="none"/>
+    <tableColumn id="25" name="Term Source REF (NCIT:C48187)" totalsRowFunction="none"/>
+    <tableColumn id="26" name="Term Accession Number (NCIT:C48187)" totalsRowFunction="none"/>
+    <tableColumn id="27" name="Output [Sample Name]" totalsRowFunction="none"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -853,10 +876,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W1"/>
+  <dimension ref="A1:AA2"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>49</v>
       </c>
@@ -925,6 +948,101 @@
       </c>
       <c r="W1" t="s">
         <v>71</v>
+      </c>
+      <c r="X1" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>73</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F2" t="s">
+        <v>76</v>
+      </c>
+      <c r="G2" t="s">
+        <v>76</v>
+      </c>
+      <c r="H2" t="s">
+        <v>76</v>
+      </c>
+      <c r="I2" t="s">
+        <v>76</v>
+      </c>
+      <c r="J2" t="s">
+        <v>76</v>
+      </c>
+      <c r="K2" t="s">
+        <v>76</v>
+      </c>
+      <c r="L2" t="s">
+        <v>76</v>
+      </c>
+      <c r="M2" t="s">
+        <v>76</v>
+      </c>
+      <c r="N2" t="s">
+        <v>76</v>
+      </c>
+      <c r="O2" t="s">
+        <v>76</v>
+      </c>
+      <c r="P2" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>76</v>
+      </c>
+      <c r="R2" t="s">
+        <v>76</v>
+      </c>
+      <c r="S2" t="s">
+        <v>76</v>
+      </c>
+      <c r="T2" t="s">
+        <v>76</v>
+      </c>
+      <c r="U2" t="s">
+        <v>76</v>
+      </c>
+      <c r="V2" t="s">
+        <v>76</v>
+      </c>
+      <c r="W2" t="s">
+        <v>76</v>
+      </c>
+      <c r="X2" t="s">
+        <v>76</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>76</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add example values for protocol columns
</commit_message>
<xml_diff>
--- a/templates/dataplant/ArrayExpress_-_Plant_sample.xlsx
+++ b/templates/dataplant/ArrayExpress_-_Plant_sample.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="95">
   <si>
     <t>TEMPLATE</t>
   </si>
@@ -243,6 +243,18 @@
   </si>
   <si>
     <t/>
+  </si>
+  <si>
+    <t>sample collection protocol</t>
+  </si>
+  <si>
+    <t>EFO</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/EFO_0005518</t>
+  </si>
+  <si>
+    <t>sample_collection.txt</t>
   </si>
   <si>
     <t>Hordeum vulgare</t>
@@ -1009,28 +1021,28 @@
         <v>76</v>
       </c>
       <c r="B2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D2" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="E2" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="F2" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="G2" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="H2" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="I2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="J2" t="s">
         <v>76</v>
@@ -1039,7 +1051,7 @@
         <v>76</v>
       </c>
       <c r="L2" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="M2" t="s">
         <v>76</v>
@@ -1048,40 +1060,40 @@
         <v>76</v>
       </c>
       <c r="O2" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="P2" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="Q2" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="R2" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="S2" t="s">
         <v>31</v>
       </c>
       <c r="T2" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="U2" t="s">
+        <v>91</v>
+      </c>
+      <c r="V2" t="s">
         <v>87</v>
       </c>
-      <c r="V2" t="s">
-        <v>83</v>
-      </c>
       <c r="W2" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="X2" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="Y2" t="s">
         <v>31</v>
       </c>
       <c r="Z2" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="AA2" t="s">
         <v>76</v>

</xml_diff>

<commit_message>
update background information and Arrayexpress template
</commit_message>
<xml_diff>
--- a/templates/dataplant/ArrayExpress_-_Plant_sample.xlsx
+++ b/templates/dataplant/ArrayExpress_-_Plant_sample.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="98">
   <si>
     <t>TEMPLATE</t>
   </si>
@@ -32,7 +32,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>1.0.3</t>
+    <t>1.0.4</t>
   </si>
   <si>
     <t>Description</t>
@@ -221,15 +221,6 @@
     <t>Term Accession Number (FOODON:00004331)</t>
   </si>
   <si>
-    <t>Factor [Experimental Factor Value]</t>
-  </si>
-  <si>
-    <t>Term Source REF (NCIT:C164386)</t>
-  </si>
-  <si>
-    <t>Term Accession Number (NCIT:C164386)</t>
-  </si>
-  <si>
     <t>Parameter [growth protocol]</t>
   </si>
   <si>
@@ -306,15 +297,6 @@
   </si>
   <si>
     <t>http://purl.obolibrary.org/obo/BAO_0000270</t>
-  </si>
-  <si>
-    <t>drought stress</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/C_24993</t>
   </si>
   <si>
     <t>plant_growth.txt</t>
@@ -379,8 +361,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" name="annotationTable" displayName="annotationTable" ref="A1:AI2" totalsRowShown="1" headerRowCount="1">
-  <autoFilter ref="A1:AI2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" name="annotationTable" displayName="annotationTable" ref="A1:AF2" totalsRowShown="1" headerRowCount="1">
+  <autoFilter ref="A1:AF2">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -413,11 +395,8 @@
     <filterColumn colId="29" hiddenButton="1"/>
     <filterColumn colId="30" hiddenButton="1"/>
     <filterColumn colId="31" hiddenButton="1"/>
-    <filterColumn colId="32" hiddenButton="1"/>
-    <filterColumn colId="33" hiddenButton="1"/>
-    <filterColumn colId="34" hiddenButton="1"/>
   </autoFilter>
-  <tableColumns count="35">
+  <tableColumns count="32">
     <tableColumn id="1" name="Input [Source Name]" totalsRowLabel="Total"/>
     <tableColumn id="2" name="Characteristic [organism]" totalsRowFunction="none"/>
     <tableColumn id="3" name="Term Source REF (OBI:0100026)" totalsRowFunction="none"/>
@@ -440,19 +419,16 @@
     <tableColumn id="20" name="Characteristic [plant material]" totalsRowFunction="none"/>
     <tableColumn id="21" name="Term Source REF (FOODON:00004331)" totalsRowFunction="none"/>
     <tableColumn id="22" name="Term Accession Number (FOODON:00004331)" totalsRowFunction="none"/>
-    <tableColumn id="23" name="Factor [Experimental Factor Value]" totalsRowFunction="none"/>
-    <tableColumn id="24" name="Term Source REF (NCIT:C164386)" totalsRowFunction="none"/>
-    <tableColumn id="25" name="Term Accession Number (NCIT:C164386)" totalsRowFunction="none"/>
-    <tableColumn id="26" name="Parameter [growth protocol]" totalsRowFunction="none"/>
-    <tableColumn id="27" name="Term Source REF (EFO:0003789)" totalsRowFunction="none"/>
-    <tableColumn id="28" name="Term Accession Number (EFO:0003789)" totalsRowFunction="none"/>
-    <tableColumn id="29" name="Parameter [sample collection protocol]" totalsRowFunction="none"/>
-    <tableColumn id="30" name="Term Source REF (EFO:0005518)" totalsRowFunction="none"/>
-    <tableColumn id="31" name="Term Accession Number (EFO:0005518)" totalsRowFunction="none"/>
-    <tableColumn id="32" name="Parameter [nucleic acid extraction protocol]" totalsRowFunction="none"/>
-    <tableColumn id="33" name="Term Source REF (EFO:0002944)" totalsRowFunction="none"/>
-    <tableColumn id="34" name="Term Accession Number (EFO:0002944)" totalsRowFunction="none"/>
-    <tableColumn id="35" name="Output [Sample Name]" totalsRowFunction="none"/>
+    <tableColumn id="23" name="Parameter [growth protocol]" totalsRowFunction="none"/>
+    <tableColumn id="24" name="Term Source REF (EFO:0003789)" totalsRowFunction="none"/>
+    <tableColumn id="25" name="Term Accession Number (EFO:0003789)" totalsRowFunction="none"/>
+    <tableColumn id="26" name="Parameter [sample collection protocol]" totalsRowFunction="none"/>
+    <tableColumn id="27" name="Term Source REF (EFO:0005518)" totalsRowFunction="none"/>
+    <tableColumn id="28" name="Term Accession Number (EFO:0005518)" totalsRowFunction="none"/>
+    <tableColumn id="29" name="Parameter [nucleic acid extraction protocol]" totalsRowFunction="none"/>
+    <tableColumn id="30" name="Term Source REF (EFO:0002944)" totalsRowFunction="none"/>
+    <tableColumn id="31" name="Term Accession Number (EFO:0002944)" totalsRowFunction="none"/>
+    <tableColumn id="32" name="Output [Sample Name]" totalsRowFunction="none"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -964,10 +940,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AI2"/>
+  <dimension ref="A1:AF2"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>47</v>
       </c>
@@ -1064,121 +1040,103 @@
       <c r="AF1" t="s">
         <v>78</v>
       </c>
-      <c r="AG1" t="s">
+    </row>
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>79</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="B2" t="s">
         <v>80</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="C2" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="D2" t="s">
         <v>82</v>
       </c>
-      <c r="B2" t="s">
+      <c r="E2" t="s">
         <v>83</v>
       </c>
-      <c r="C2" t="s">
+      <c r="F2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G2" t="s">
+        <v>79</v>
+      </c>
+      <c r="H2" t="s">
         <v>84</v>
       </c>
-      <c r="D2" t="s">
+      <c r="I2" t="s">
+        <v>79</v>
+      </c>
+      <c r="J2" t="s">
+        <v>79</v>
+      </c>
+      <c r="K2" t="s">
         <v>85</v>
       </c>
-      <c r="E2" t="s">
+      <c r="L2" t="s">
         <v>86</v>
       </c>
-      <c r="F2" t="s">
-        <v>82</v>
-      </c>
-      <c r="G2" t="s">
-        <v>82</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="M2" t="s">
         <v>87</v>
       </c>
-      <c r="I2" t="s">
-        <v>82</v>
-      </c>
-      <c r="J2" t="s">
-        <v>82</v>
-      </c>
-      <c r="K2" t="s">
+      <c r="N2" t="s">
         <v>88</v>
-      </c>
-      <c r="L2" t="s">
-        <v>89</v>
-      </c>
-      <c r="M2" t="s">
-        <v>90</v>
-      </c>
-      <c r="N2" t="s">
-        <v>91</v>
       </c>
       <c r="O2" t="s">
         <v>29</v>
       </c>
       <c r="P2" t="s">
+        <v>89</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>90</v>
+      </c>
+      <c r="R2" t="s">
+        <v>86</v>
+      </c>
+      <c r="S2" t="s">
+        <v>91</v>
+      </c>
+      <c r="T2" t="s">
         <v>92</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="U2" t="s">
         <v>93</v>
       </c>
-      <c r="R2" t="s">
-        <v>89</v>
-      </c>
-      <c r="S2" t="s">
+      <c r="V2" t="s">
         <v>94</v>
       </c>
-      <c r="T2" t="s">
+      <c r="W2" t="s">
         <v>95</v>
       </c>
-      <c r="U2" t="s">
+      <c r="X2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z2" t="s">
         <v>96</v>
       </c>
-      <c r="V2" t="s">
+      <c r="AA2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AC2" t="s">
         <v>97</v>
       </c>
-      <c r="W2" t="s">
-        <v>98</v>
-      </c>
-      <c r="X2" t="s">
-        <v>99</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>100</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>101</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>82</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>82</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>102</v>
-      </c>
       <c r="AD2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="AE2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="AF2" t="s">
-        <v>103</v>
-      </c>
-      <c r="AG2" t="s">
-        <v>82</v>
-      </c>
-      <c r="AH2" t="s">
-        <v>82</v>
-      </c>
-      <c r="AI2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>